<commit_message>
Correzione Report Check List
Applicate le correzioni sul file Report Check List per come da vostre indicazioni.
Avevo messo erroneamente KO al caso 4.
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111RBSOFTWARECENTERSRLXX/RBSoftware/WGesLaAn/1/report-checklist.xlsx
+++ b/GATEWAY/S1#111RBSOFTWARECENTERSRLXX/RBSoftware/WGesLaAn/1/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VB6\WGesLaAn\Documenti\FSE\FSE 2.0\Accreditamento 2025\INVIO\S1#111#RBSOFTWARECENTERSRLXX\RBSoftware\WGesLaAn\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AA2DED-02C7-41C6-8331-004A840778CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7D97D1-F5FA-4D4F-B4A7-0991D8D38D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="0" windowWidth="28305" windowHeight="8415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="150" yWindow="0" windowWidth="28305" windowHeight="8415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1626" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1630" uniqueCount="656">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -4587,7 +4587,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="S191" sqref="S191"/>
+      <selection pane="bottomRight" activeCell="T31" sqref="T31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4924,7 +4924,7 @@
       <c r="U10" s="39"/>
       <c r="V10" s="40"/>
       <c r="W10" s="38" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="270.75" thickBot="1">
@@ -5940,7 +5940,7 @@
       <c r="R31" s="38"/>
       <c r="S31" s="38"/>
       <c r="T31" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U31" s="39"/>
       <c r="V31" s="40"/>
@@ -6100,7 +6100,7 @@
       <c r="R35" s="38"/>
       <c r="S35" s="38"/>
       <c r="T35" s="38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="U35" s="39"/>
       <c r="V35" s="40"/>
@@ -6141,8 +6141,12 @@
       </c>
       <c r="K36" s="38"/>
       <c r="L36" s="38"/>
-      <c r="M36" s="38"/>
-      <c r="N36" s="38"/>
+      <c r="M36" s="38" t="s">
+        <v>228</v>
+      </c>
+      <c r="N36" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O36" s="38"/>
       <c r="P36" s="38"/>
       <c r="Q36" s="38"/>
@@ -9832,7 +9836,9 @@
       <c r="M122" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N122" s="38"/>
+      <c r="N122" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O122" s="38"/>
       <c r="P122" s="38"/>
       <c r="Q122" s="38"/>
@@ -9883,7 +9889,9 @@
       <c r="M123" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="N123" s="38"/>
+      <c r="N123" s="38" t="s">
+        <v>228</v>
+      </c>
       <c r="O123" s="38"/>
       <c r="P123" s="38"/>
       <c r="Q123" s="38"/>
@@ -19281,6 +19289,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19538,28 +19567,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19578,31 +19611,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>

<commit_message>
Aggiornata Check List con casi mancanti
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111RBSOFTWARECENTERSRLXX/RBSoftware/WGesLaAn/1/report-checklist.xlsx
+++ b/GATEWAY/S1#111RBSOFTWARECENTERSRLXX/RBSoftware/WGesLaAn/1/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VB6\WGesLaAn\Documenti\FSE\FSE 2.0\Accreditamento 2025\INVIO\S1#111#RBSOFTWARECENTERSRLXX\RBSoftware\WGesLaAn\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7D97D1-F5FA-4D4F-B4A7-0991D8D38D1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0BDBD79-69DC-465A-B0C9-AC887CEFA921}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="150" yWindow="0" windowWidth="28305" windowHeight="8415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="225" yWindow="0" windowWidth="28305" windowHeight="8415" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -1711,12 +1711,6 @@
     <t>R.B. Software Center S.r.l.</t>
   </si>
   <si>
-    <t>2025-10-29T05:09:24Z</t>
-  </si>
-  <si>
-    <t>6f893c73d651f9ae58208b206fff8809</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
@@ -1725,12 +1719,6 @@
   <si>
     <t>Il controllo sulla generazione del Token viene fatto a monte prima della procedura di validazione. In caso di errore viene visualizzato un messaggio a video riportante il tipo di errore.
 Il verificarsi di tale tipo di errore  dopo esser stato notificato consente all’utente di proseguire  con il processo e produrre il documento; il documento sarà però gestito tramite una coda e reinviato a valle della risoluzione dell’errore.</t>
-  </si>
-  <si>
-    <t>7e97c4cf0ec943fe48df802691e7d434</t>
-  </si>
-  <si>
-    <t>2025-10-29T05:13:04Z</t>
   </si>
   <si>
     <t>Il campo action_id non è corretto</t>
@@ -1926,18 +1914,6 @@
     <t>Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: X]</t>
   </si>
   <si>
-    <t>2025-10-29T08:35:48Z</t>
-  </si>
-  <si>
-    <t>c2d880de6f6aed5eabfea55503b92816</t>
-  </si>
-  <si>
-    <t>2025-10-29T08:40:16Z</t>
-  </si>
-  <si>
-    <t>d85fb59ccc03c632c844e890bffa0b23</t>
-  </si>
-  <si>
     <t>codice fiscale 'prvprv00a41h501w' cittadino ed operatore: 16 cifre [A-Z0-9]{16}</t>
   </si>
   <si>
@@ -2155,18 +2131,6 @@
   <si>
     <t>Errore vocabolario.
 Almeno uno dei seguenti vocaboli non è censito: [CodeSystem: 2.16.840.1.113883.5.7 v2.1.0, Codes: RX]</t>
-  </si>
-  <si>
-    <t>2025-10-30T10:23:08Z</t>
-  </si>
-  <si>
-    <t>639d743f10b595213dee805c17b4c839</t>
-  </si>
-  <si>
-    <t>2025-10-30T10:25:01Z</t>
-  </si>
-  <si>
-    <t>1b73e93c6cabb089c0507ea86316ab43</t>
   </si>
   <si>
     <t>2025-10-30T10:35:29Z</t>
@@ -2422,6 +2386,42 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.e099f584cc9eb012b53a9bea661f73bf22cf1bafe2c8d86a005df6f7fa7a0242.d23332be6e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-11-04T03:52:26Z</t>
+  </si>
+  <si>
+    <t>40c12b6c72eb374e6567ab04b38e513c</t>
+  </si>
+  <si>
+    <t>2025-11-04T03:57:03Z</t>
+  </si>
+  <si>
+    <t>d8e9ae6cad4b44b59b528f80528ccca1</t>
+  </si>
+  <si>
+    <t>2025-11-04T04:01:21Z</t>
+  </si>
+  <si>
+    <t>510166072f2a2242e3a9f2062ab36f7f</t>
+  </si>
+  <si>
+    <t>2025-11-04T04:04:48Z</t>
+  </si>
+  <si>
+    <t>142a6c73e1c922b5806c207fbc6022ed</t>
+  </si>
+  <si>
+    <t>2025-11-04T04:07:30Z</t>
+  </si>
+  <si>
+    <t>c240ba19a98707e0f7ef91a65358af28</t>
+  </si>
+  <si>
+    <t>2025-11-04T04:10:24Z</t>
+  </si>
+  <si>
+    <t>8cefdef1c6422095093870ed5bb45bc0</t>
   </si>
 </sst>
 </file>
@@ -4587,7 +4587,7 @@
       <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="T31" sqref="T31"/>
+      <selection pane="bottomRight" activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4662,7 +4662,7 @@
       </c>
       <c r="B3" s="73"/>
       <c r="C3" s="80" t="s">
-        <v>627</v>
+        <v>615</v>
       </c>
       <c r="D3" s="79"/>
       <c r="F3" s="6"/>
@@ -4688,7 +4688,7 @@
       <c r="A4" s="74"/>
       <c r="B4" s="75"/>
       <c r="C4" s="80" t="s">
-        <v>628</v>
+        <v>616</v>
       </c>
       <c r="D4" s="79"/>
       <c r="E4" s="4"/>
@@ -4715,7 +4715,7 @@
       <c r="A5" s="76"/>
       <c r="B5" s="77"/>
       <c r="C5" s="80" t="s">
-        <v>629</v>
+        <v>617</v>
       </c>
       <c r="D5" s="79"/>
       <c r="F5" s="6"/>
@@ -4944,16 +4944,16 @@
         <v>43</v>
       </c>
       <c r="F11" s="36">
-        <v>45959</v>
+        <v>45965</v>
       </c>
       <c r="G11" s="37" t="s">
+        <v>644</v>
+      </c>
+      <c r="H11" s="37" t="s">
+        <v>645</v>
+      </c>
+      <c r="I11" s="42" t="s">
         <v>441</v>
-      </c>
-      <c r="H11" s="37" t="s">
-        <v>442</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>443</v>
       </c>
       <c r="J11" s="38" t="s">
         <v>64</v>
@@ -4967,7 +4967,7 @@
         <v>64</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="P11" s="38" t="s">
         <v>64</v>
@@ -4975,7 +4975,7 @@
       <c r="Q11" s="38"/>
       <c r="R11" s="38"/>
       <c r="S11" s="47" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T11" s="38" t="s">
         <v>226</v>
@@ -5003,16 +5003,16 @@
         <v>55</v>
       </c>
       <c r="F12" s="36">
-        <v>45959</v>
+        <v>45965</v>
       </c>
       <c r="G12" s="37" t="s">
-        <v>447</v>
+        <v>646</v>
       </c>
       <c r="H12" s="37" t="s">
-        <v>446</v>
+        <v>647</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J12" s="38" t="s">
         <v>64</v>
@@ -5026,7 +5026,7 @@
         <v>64</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="P12" s="38" t="s">
         <v>64</v>
@@ -5034,7 +5034,7 @@
       <c r="Q12" s="38"/>
       <c r="R12" s="38"/>
       <c r="S12" s="49" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T12" s="38" t="s">
         <v>226</v>
@@ -5114,7 +5114,7 @@
         <v>64</v>
       </c>
       <c r="O14" s="50" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="P14" s="38" t="s">
         <v>64</v>
@@ -5122,7 +5122,7 @@
       <c r="Q14" s="38"/>
       <c r="R14" s="38"/>
       <c r="S14" s="51" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="T14" s="38" t="s">
         <v>226</v>
@@ -5155,13 +5155,13 @@
         <v>45959</v>
       </c>
       <c r="G15" s="37" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="H15" s="37" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="I15" s="42" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="J15" s="38" t="s">
         <v>64</v>
@@ -5175,7 +5175,7 @@
         <v>64</v>
       </c>
       <c r="O15" s="38" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="P15" s="38" t="s">
         <v>64</v>
@@ -5183,7 +5183,7 @@
       <c r="Q15" s="38"/>
       <c r="R15" s="38"/>
       <c r="S15" s="52" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="T15" s="38" t="s">
         <v>226</v>
@@ -5325,13 +5325,13 @@
         <v>45959</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="I19" s="42" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="J19" s="38" t="s">
         <v>64</v>
@@ -5345,7 +5345,7 @@
         <v>64</v>
       </c>
       <c r="O19" s="53" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="P19" s="38" t="s">
         <v>64</v>
@@ -5353,7 +5353,7 @@
       <c r="Q19" s="38"/>
       <c r="R19" s="38"/>
       <c r="S19" s="54" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T19" s="38" t="s">
         <v>226</v>
@@ -5384,13 +5384,13 @@
         <v>45959</v>
       </c>
       <c r="G20" s="37" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="I20" s="42" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="J20" s="38" t="s">
         <v>64</v>
@@ -5404,7 +5404,7 @@
         <v>64</v>
       </c>
       <c r="O20" s="55" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="P20" s="38" t="s">
         <v>64</v>
@@ -5412,7 +5412,7 @@
       <c r="Q20" s="38"/>
       <c r="R20" s="38"/>
       <c r="S20" s="56" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T20" s="38" t="s">
         <v>226</v>
@@ -5480,13 +5480,13 @@
         <v>45959</v>
       </c>
       <c r="G22" s="37" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H22" s="37" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="I22" s="42" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="J22" s="38" t="s">
         <v>64</v>
@@ -5500,7 +5500,7 @@
         <v>64</v>
       </c>
       <c r="O22" s="57" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="P22" s="38" t="s">
         <v>64</v>
@@ -5508,7 +5508,7 @@
       <c r="Q22" s="38"/>
       <c r="R22" s="38"/>
       <c r="S22" s="58" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T22" s="38" t="s">
         <v>226</v>
@@ -5539,13 +5539,13 @@
         <v>45959</v>
       </c>
       <c r="G23" s="37" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="I23" s="42" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="J23" s="38" t="s">
         <v>64</v>
@@ -5559,7 +5559,7 @@
         <v>64</v>
       </c>
       <c r="O23" s="38" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="P23" s="38" t="s">
         <v>64</v>
@@ -5567,7 +5567,7 @@
       <c r="Q23" s="38"/>
       <c r="R23" s="38"/>
       <c r="S23" s="59" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T23" s="38" t="s">
         <v>226</v>
@@ -5709,13 +5709,13 @@
         <v>45959</v>
       </c>
       <c r="G27" s="37" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="H27" s="37" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="I27" s="42" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="J27" s="38" t="s">
         <v>64</v>
@@ -5729,7 +5729,7 @@
         <v>64</v>
       </c>
       <c r="O27" s="38" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="P27" s="38" t="s">
         <v>64</v>
@@ -5737,7 +5737,7 @@
       <c r="Q27" s="38"/>
       <c r="R27" s="38"/>
       <c r="S27" s="60" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="T27" s="38" t="s">
         <v>226</v>
@@ -5768,13 +5768,13 @@
         <v>45959</v>
       </c>
       <c r="G28" s="37" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="H28" s="37" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="I28" s="42" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="J28" s="38" t="s">
         <v>64</v>
@@ -5788,7 +5788,7 @@
         <v>64</v>
       </c>
       <c r="O28" s="38" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="P28" s="38" t="s">
         <v>64</v>
@@ -5796,7 +5796,7 @@
       <c r="Q28" s="38"/>
       <c r="R28" s="38"/>
       <c r="S28" s="61" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="T28" s="38" t="s">
         <v>226</v>
@@ -5839,7 +5839,7 @@
       <c r="S29" s="38"/>
       <c r="T29" s="38"/>
       <c r="U29" s="39" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="V29" s="40"/>
       <c r="W29" s="38" t="s">
@@ -5866,13 +5866,13 @@
         <v>45959</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="I30" s="42" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="J30" s="38" t="s">
         <v>64</v>
@@ -5886,7 +5886,7 @@
         <v>64</v>
       </c>
       <c r="O30" s="38" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="P30" s="38" t="s">
         <v>64</v>
@@ -5894,7 +5894,7 @@
       <c r="Q30" s="62"/>
       <c r="R30" s="38"/>
       <c r="S30" s="63" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T30" s="38" t="s">
         <v>226</v>
@@ -5980,7 +5980,7 @@
       <c r="S32" s="38"/>
       <c r="T32" s="38"/>
       <c r="U32" s="39" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="V32" s="40"/>
       <c r="W32" s="38" t="s">
@@ -6019,7 +6019,7 @@
       <c r="S33" s="38"/>
       <c r="T33" s="38"/>
       <c r="U33" s="39" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="V33" s="40"/>
       <c r="W33" s="38" t="s">
@@ -6058,7 +6058,7 @@
       <c r="S34" s="38"/>
       <c r="T34" s="38"/>
       <c r="U34" s="39" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="V34" s="40"/>
       <c r="W34" s="38" t="s">
@@ -6128,13 +6128,13 @@
         <v>45959</v>
       </c>
       <c r="G36" s="37" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="H36" s="37" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="I36" s="42" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="J36" s="38" t="s">
         <v>64</v>
@@ -6181,13 +6181,13 @@
         <v>45959</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="H37" s="35" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="I37" s="45" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="J37" s="38" t="s">
         <v>64</v>
@@ -6201,7 +6201,7 @@
         <v>64</v>
       </c>
       <c r="O37" s="38" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="P37" s="38" t="s">
         <v>64</v>
@@ -6209,7 +6209,7 @@
       <c r="Q37" s="38"/>
       <c r="R37" s="38"/>
       <c r="S37" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T37" s="38" t="s">
         <v>226</v>
@@ -6240,13 +6240,13 @@
         <v>45959</v>
       </c>
       <c r="G38" s="37" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="H38" s="37" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="I38" s="42" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="J38" s="38" t="s">
         <v>64</v>
@@ -6260,7 +6260,7 @@
         <v>64</v>
       </c>
       <c r="O38" s="38" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="P38" s="38" t="s">
         <v>64</v>
@@ -6268,7 +6268,7 @@
       <c r="Q38" s="38"/>
       <c r="R38" s="38"/>
       <c r="S38" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T38" s="38" t="s">
         <v>226</v>
@@ -6888,16 +6888,16 @@
         <v>43</v>
       </c>
       <c r="F55" s="36">
-        <v>45959</v>
+        <v>45965</v>
       </c>
       <c r="G55" s="37" t="s">
-        <v>501</v>
+        <v>650</v>
       </c>
       <c r="H55" s="37" t="s">
-        <v>502</v>
+        <v>651</v>
       </c>
       <c r="I55" s="42" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J55" s="38" t="s">
         <v>64</v>
@@ -6911,7 +6911,7 @@
         <v>64</v>
       </c>
       <c r="O55" s="64" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="P55" s="38" t="s">
         <v>64</v>
@@ -6919,7 +6919,7 @@
       <c r="Q55" s="38"/>
       <c r="R55" s="38"/>
       <c r="S55" s="65" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T55" s="38" t="s">
         <v>226</v>
@@ -6947,16 +6947,16 @@
         <v>55</v>
       </c>
       <c r="F56" s="36">
-        <v>45959</v>
+        <v>45965</v>
       </c>
       <c r="G56" s="37" t="s">
-        <v>503</v>
+        <v>648</v>
       </c>
       <c r="H56" s="37" t="s">
-        <v>504</v>
+        <v>649</v>
       </c>
       <c r="I56" s="42" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J56" s="38" t="s">
         <v>64</v>
@@ -6970,7 +6970,7 @@
         <v>64</v>
       </c>
       <c r="O56" s="64" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="P56" s="38" t="s">
         <v>64</v>
@@ -6978,7 +6978,7 @@
       <c r="Q56" s="38"/>
       <c r="R56" s="38"/>
       <c r="S56" s="65" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T56" s="38" t="s">
         <v>226</v>
@@ -7021,7 +7021,7 @@
         <v>64</v>
       </c>
       <c r="O57" s="64" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="P57" s="38" t="s">
         <v>64</v>
@@ -7029,7 +7029,7 @@
       <c r="Q57" s="38"/>
       <c r="R57" s="38"/>
       <c r="S57" s="65" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="T57" s="38" t="s">
         <v>226</v>
@@ -7062,13 +7062,13 @@
         <v>45959</v>
       </c>
       <c r="G58" s="37" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="H58" s="37" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="I58" s="42" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="J58" s="38" t="s">
         <v>64</v>
@@ -7082,7 +7082,7 @@
         <v>64</v>
       </c>
       <c r="O58" s="38" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="P58" s="38" t="s">
         <v>64</v>
@@ -7090,7 +7090,7 @@
       <c r="Q58" s="38"/>
       <c r="R58" s="38"/>
       <c r="S58" s="65" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="T58" s="38" t="s">
         <v>226</v>
@@ -7121,13 +7121,13 @@
         <v>45959</v>
       </c>
       <c r="G59" s="37" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="H59" s="37" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="I59" s="42" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="J59" s="38" t="s">
         <v>64</v>
@@ -7141,7 +7141,7 @@
         <v>64</v>
       </c>
       <c r="O59" s="64" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="P59" s="38" t="s">
         <v>64</v>
@@ -7149,7 +7149,7 @@
       <c r="Q59" s="38"/>
       <c r="R59" s="38"/>
       <c r="S59" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T59" s="38" t="s">
         <v>226</v>
@@ -7180,13 +7180,13 @@
         <v>45959</v>
       </c>
       <c r="G60" s="37" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="H60" s="37" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="I60" s="42" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="J60" s="38" t="s">
         <v>64</v>
@@ -7200,7 +7200,7 @@
         <v>64</v>
       </c>
       <c r="O60" s="64" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="P60" s="38" t="s">
         <v>64</v>
@@ -7208,7 +7208,7 @@
       <c r="Q60" s="38"/>
       <c r="R60" s="38"/>
       <c r="S60" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T60" s="38" t="s">
         <v>226</v>
@@ -7239,13 +7239,13 @@
         <v>45959</v>
       </c>
       <c r="G61" s="37" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="H61" s="37" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="I61" s="42" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="J61" s="38" t="s">
         <v>64</v>
@@ -7259,7 +7259,7 @@
         <v>64</v>
       </c>
       <c r="O61" s="64" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="P61" s="38" t="s">
         <v>64</v>
@@ -7267,7 +7267,7 @@
       <c r="Q61" s="38"/>
       <c r="R61" s="38"/>
       <c r="S61" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T61" s="38" t="s">
         <v>226</v>
@@ -7298,13 +7298,13 @@
         <v>45959</v>
       </c>
       <c r="G62" s="37" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="H62" s="37" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="I62" s="42" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="J62" s="38" t="s">
         <v>64</v>
@@ -7318,7 +7318,7 @@
         <v>64</v>
       </c>
       <c r="O62" s="38" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="P62" s="38" t="s">
         <v>64</v>
@@ -7326,7 +7326,7 @@
       <c r="Q62" s="38"/>
       <c r="R62" s="38"/>
       <c r="S62" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T62" s="38" t="s">
         <v>226</v>
@@ -7357,13 +7357,13 @@
         <v>45959</v>
       </c>
       <c r="G63" s="37" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
       <c r="H63" s="37" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="I63" s="42" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="J63" s="38" t="s">
         <v>64</v>
@@ -7377,7 +7377,7 @@
         <v>64</v>
       </c>
       <c r="O63" s="38" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
       <c r="P63" s="38" t="s">
         <v>64</v>
@@ -7385,7 +7385,7 @@
       <c r="Q63" s="38"/>
       <c r="R63" s="38"/>
       <c r="S63" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T63" s="38" t="s">
         <v>226</v>
@@ -7416,13 +7416,13 @@
         <v>45959</v>
       </c>
       <c r="G64" s="37" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
       <c r="H64" s="37" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="I64" s="42" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="J64" s="38" t="s">
         <v>64</v>
@@ -7436,7 +7436,7 @@
         <v>64</v>
       </c>
       <c r="O64" s="38" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="P64" s="38" t="s">
         <v>64</v>
@@ -7444,7 +7444,7 @@
       <c r="Q64" s="38"/>
       <c r="R64" s="38"/>
       <c r="S64" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T64" s="38" t="s">
         <v>226</v>
@@ -7475,13 +7475,13 @@
         <v>45959</v>
       </c>
       <c r="G65" s="37" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="H65" s="37" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="I65" s="42" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="J65" s="38" t="s">
         <v>64</v>
@@ -7495,7 +7495,7 @@
         <v>64</v>
       </c>
       <c r="O65" s="38" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="P65" s="38" t="s">
         <v>64</v>
@@ -7503,7 +7503,7 @@
       <c r="Q65" s="38"/>
       <c r="R65" s="38"/>
       <c r="S65" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T65" s="38" t="s">
         <v>226</v>
@@ -7534,13 +7534,13 @@
         <v>45959</v>
       </c>
       <c r="G66" s="37" t="s">
-        <v>534</v>
+        <v>526</v>
       </c>
       <c r="H66" s="37" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
       <c r="I66" s="42" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="J66" s="38" t="s">
         <v>64</v>
@@ -7554,7 +7554,7 @@
         <v>64</v>
       </c>
       <c r="O66" s="38" t="s">
-        <v>537</v>
+        <v>529</v>
       </c>
       <c r="P66" s="38" t="s">
         <v>64</v>
@@ -7562,7 +7562,7 @@
       <c r="Q66" s="38"/>
       <c r="R66" s="38"/>
       <c r="S66" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T66" s="38" t="s">
         <v>226</v>
@@ -7593,13 +7593,13 @@
         <v>45959</v>
       </c>
       <c r="G67" s="37" t="s">
-        <v>538</v>
+        <v>530</v>
       </c>
       <c r="H67" s="37" t="s">
-        <v>539</v>
+        <v>531</v>
       </c>
       <c r="I67" s="42" t="s">
-        <v>540</v>
+        <v>532</v>
       </c>
       <c r="J67" s="38" t="s">
         <v>64</v>
@@ -7613,7 +7613,7 @@
         <v>64</v>
       </c>
       <c r="O67" s="38" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
       <c r="P67" s="38" t="s">
         <v>64</v>
@@ -7621,7 +7621,7 @@
       <c r="Q67" s="38"/>
       <c r="R67" s="38"/>
       <c r="S67" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T67" s="38" t="s">
         <v>226</v>
@@ -7652,13 +7652,13 @@
         <v>45959</v>
       </c>
       <c r="G68" s="37" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="H68" s="37" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
       <c r="I68" s="42" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="J68" s="38" t="s">
         <v>64</v>
@@ -7672,7 +7672,7 @@
         <v>64</v>
       </c>
       <c r="O68" s="38" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="P68" s="38" t="s">
         <v>64</v>
@@ -7680,7 +7680,7 @@
       <c r="Q68" s="38"/>
       <c r="R68" s="38"/>
       <c r="S68" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T68" s="38" t="s">
         <v>226</v>
@@ -9450,13 +9450,13 @@
         <v>45959</v>
       </c>
       <c r="G116" s="37" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="H116" s="37" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="I116" s="42" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="J116" s="38" t="s">
         <v>64</v>
@@ -9470,7 +9470,7 @@
         <v>64</v>
       </c>
       <c r="O116" s="38" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="P116" s="38" t="s">
         <v>64</v>
@@ -9478,7 +9478,7 @@
       <c r="Q116" s="38"/>
       <c r="R116" s="38"/>
       <c r="S116" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T116" s="38" t="s">
         <v>226</v>
@@ -9509,13 +9509,13 @@
         <v>45959</v>
       </c>
       <c r="G117" s="37" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="H117" s="37" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="I117" s="42" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="J117" s="38" t="s">
         <v>64</v>
@@ -9529,7 +9529,7 @@
         <v>64</v>
       </c>
       <c r="O117" s="38" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="P117" s="38" t="s">
         <v>64</v>
@@ -9537,7 +9537,7 @@
       <c r="Q117" s="38"/>
       <c r="R117" s="38"/>
       <c r="S117" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T117" s="38" t="s">
         <v>226</v>
@@ -9568,13 +9568,13 @@
         <v>45959</v>
       </c>
       <c r="G118" s="37" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="H118" s="37" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="I118" s="42" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="J118" s="38" t="s">
         <v>64</v>
@@ -9588,7 +9588,7 @@
         <v>64</v>
       </c>
       <c r="O118" s="38" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="P118" s="38" t="s">
         <v>64</v>
@@ -9600,7 +9600,7 @@
         <v>64</v>
       </c>
       <c r="S118" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T118" s="38" t="s">
         <v>226</v>
@@ -9631,13 +9631,13 @@
         <v>45960</v>
       </c>
       <c r="G119" s="37" t="s">
-        <v>558</v>
+        <v>550</v>
       </c>
       <c r="H119" s="37" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="I119" s="42" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="J119" s="38" t="s">
         <v>64</v>
@@ -9651,7 +9651,7 @@
         <v>64</v>
       </c>
       <c r="O119" s="38" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="P119" s="38" t="s">
         <v>64</v>
@@ -9663,7 +9663,7 @@
         <v>64</v>
       </c>
       <c r="S119" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T119" s="38" t="s">
         <v>226</v>
@@ -9694,13 +9694,13 @@
         <v>45960</v>
       </c>
       <c r="G120" s="37" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="H120" s="37" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
       <c r="I120" s="42" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="J120" s="38" t="s">
         <v>64</v>
@@ -9714,7 +9714,7 @@
         <v>64</v>
       </c>
       <c r="O120" s="38" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
       <c r="P120" s="38" t="s">
         <v>64</v>
@@ -9726,7 +9726,7 @@
         <v>64</v>
       </c>
       <c r="S120" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T120" s="38" t="s">
         <v>226</v>
@@ -9757,13 +9757,13 @@
         <v>45960</v>
       </c>
       <c r="G121" s="35" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="H121" s="35" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="I121" s="45" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="J121" s="38" t="s">
         <v>64</v>
@@ -9777,7 +9777,7 @@
         <v>64</v>
       </c>
       <c r="O121" s="38" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="P121" s="38" t="s">
         <v>64</v>
@@ -9789,7 +9789,7 @@
         <v>64</v>
       </c>
       <c r="S121" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T121" s="38" t="s">
         <v>226</v>
@@ -9820,13 +9820,13 @@
         <v>45960</v>
       </c>
       <c r="G122" s="37" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="H122" s="37" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="I122" s="42" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
       <c r="J122" s="38" t="s">
         <v>64</v>
@@ -9873,13 +9873,13 @@
         <v>45960</v>
       </c>
       <c r="G123" s="37" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="H123" s="37" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="I123" s="42" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="J123" s="38" t="s">
         <v>64</v>
@@ -9926,13 +9926,13 @@
         <v>45960</v>
       </c>
       <c r="G124" s="37" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="H124" s="37" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="I124" s="42" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="J124" s="38" t="s">
         <v>64</v>
@@ -9946,7 +9946,7 @@
         <v>64</v>
       </c>
       <c r="O124" s="38" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="P124" s="38" t="s">
         <v>64</v>
@@ -9958,7 +9958,7 @@
         <v>64</v>
       </c>
       <c r="S124" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T124" s="38" t="s">
         <v>226</v>
@@ -9986,16 +9986,16 @@
         <v>43</v>
       </c>
       <c r="F125" s="37">
-        <v>45960</v>
+        <v>45965</v>
       </c>
       <c r="G125" s="37" t="s">
-        <v>576</v>
+        <v>652</v>
       </c>
       <c r="H125" s="37" t="s">
-        <v>577</v>
+        <v>653</v>
       </c>
       <c r="I125" s="42" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J125" s="38" t="s">
         <v>64</v>
@@ -10009,7 +10009,7 @@
         <v>64</v>
       </c>
       <c r="O125" s="64" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="P125" s="38" t="s">
         <v>64</v>
@@ -10017,7 +10017,7 @@
       <c r="Q125" s="38"/>
       <c r="R125" s="38"/>
       <c r="S125" s="65" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T125" s="38" t="s">
         <v>226</v>
@@ -10045,16 +10045,16 @@
         <v>55</v>
       </c>
       <c r="F126" s="37">
-        <v>45960</v>
+        <v>45965</v>
       </c>
       <c r="G126" s="37" t="s">
-        <v>578</v>
+        <v>654</v>
       </c>
       <c r="H126" s="37" t="s">
-        <v>579</v>
+        <v>655</v>
       </c>
       <c r="I126" s="42" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J126" s="38" t="s">
         <v>64</v>
@@ -10068,7 +10068,7 @@
         <v>64</v>
       </c>
       <c r="O126" s="64" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="P126" s="38" t="s">
         <v>64</v>
@@ -10076,7 +10076,7 @@
       <c r="Q126" s="38"/>
       <c r="R126" s="38"/>
       <c r="S126" s="65" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="T126" s="38" t="s">
         <v>226</v>
@@ -10119,7 +10119,7 @@
         <v>64</v>
       </c>
       <c r="O127" s="64" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="P127" s="38" t="s">
         <v>64</v>
@@ -10127,7 +10127,7 @@
       <c r="Q127" s="38"/>
       <c r="R127" s="38"/>
       <c r="S127" s="65" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="T127" s="38" t="s">
         <v>226</v>
@@ -10160,13 +10160,13 @@
         <v>45960</v>
       </c>
       <c r="G128" s="37" t="s">
-        <v>580</v>
+        <v>568</v>
       </c>
       <c r="H128" s="37" t="s">
-        <v>581</v>
+        <v>569</v>
       </c>
       <c r="I128" s="42" t="s">
-        <v>582</v>
+        <v>570</v>
       </c>
       <c r="J128" s="38" t="s">
         <v>64</v>
@@ -10180,7 +10180,7 @@
         <v>64</v>
       </c>
       <c r="O128" s="38" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="P128" s="38" t="s">
         <v>64</v>
@@ -10188,7 +10188,7 @@
       <c r="Q128" s="38"/>
       <c r="R128" s="38"/>
       <c r="S128" s="65" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="T128" s="38" t="s">
         <v>226</v>
@@ -10219,13 +10219,13 @@
         <v>45960</v>
       </c>
       <c r="G129" s="37" t="s">
-        <v>583</v>
+        <v>571</v>
       </c>
       <c r="H129" s="37" t="s">
-        <v>584</v>
+        <v>572</v>
       </c>
       <c r="I129" s="42" t="s">
-        <v>585</v>
+        <v>573</v>
       </c>
       <c r="J129" s="38" t="s">
         <v>64</v>
@@ -10239,7 +10239,7 @@
         <v>64</v>
       </c>
       <c r="O129" s="64" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="P129" s="38" t="s">
         <v>64</v>
@@ -10247,7 +10247,7 @@
       <c r="Q129" s="38"/>
       <c r="R129" s="38"/>
       <c r="S129" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T129" s="38" t="s">
         <v>226</v>
@@ -10278,13 +10278,13 @@
         <v>45960</v>
       </c>
       <c r="G130" s="37" t="s">
-        <v>588</v>
+        <v>576</v>
       </c>
       <c r="H130" s="37" t="s">
-        <v>587</v>
+        <v>575</v>
       </c>
       <c r="I130" s="42" t="s">
-        <v>586</v>
+        <v>574</v>
       </c>
       <c r="J130" s="38" t="s">
         <v>64</v>
@@ -10298,7 +10298,7 @@
         <v>64</v>
       </c>
       <c r="O130" s="64" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="P130" s="38" t="s">
         <v>64</v>
@@ -10306,7 +10306,7 @@
       <c r="Q130" s="38"/>
       <c r="R130" s="38"/>
       <c r="S130" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T130" s="38" t="s">
         <v>226</v>
@@ -10892,13 +10892,13 @@
         <v>45960</v>
       </c>
       <c r="G146" s="37" t="s">
-        <v>591</v>
+        <v>579</v>
       </c>
       <c r="H146" s="37" t="s">
-        <v>589</v>
+        <v>577</v>
       </c>
       <c r="I146" s="42" t="s">
-        <v>590</v>
+        <v>578</v>
       </c>
       <c r="J146" s="38" t="s">
         <v>64</v>
@@ -10912,7 +10912,7 @@
         <v>64</v>
       </c>
       <c r="O146" s="64" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="P146" s="38" t="s">
         <v>64</v>
@@ -10920,7 +10920,7 @@
       <c r="Q146" s="38"/>
       <c r="R146" s="38"/>
       <c r="S146" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T146" s="38" t="s">
         <v>226</v>
@@ -10951,13 +10951,13 @@
         <v>45960</v>
       </c>
       <c r="G147" s="37" t="s">
-        <v>593</v>
+        <v>581</v>
       </c>
       <c r="H147" s="37" t="s">
-        <v>594</v>
+        <v>582</v>
       </c>
       <c r="I147" s="42" t="s">
-        <v>595</v>
+        <v>583</v>
       </c>
       <c r="J147" s="38" t="s">
         <v>64</v>
@@ -10971,7 +10971,7 @@
         <v>64</v>
       </c>
       <c r="O147" s="38" t="s">
-        <v>592</v>
+        <v>580</v>
       </c>
       <c r="P147" s="38" t="s">
         <v>64</v>
@@ -10979,7 +10979,7 @@
       <c r="Q147" s="38"/>
       <c r="R147" s="38"/>
       <c r="S147" s="65" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="T147" s="38" t="s">
         <v>226</v>
@@ -11676,13 +11676,13 @@
         <v>45960</v>
       </c>
       <c r="G166" s="37" t="s">
-        <v>598</v>
+        <v>586</v>
       </c>
       <c r="H166" s="37" t="s">
-        <v>596</v>
+        <v>584</v>
       </c>
       <c r="I166" s="42" t="s">
-        <v>597</v>
+        <v>585</v>
       </c>
       <c r="J166" s="38" t="s">
         <v>64</v>
@@ -11696,7 +11696,7 @@
         <v>64</v>
       </c>
       <c r="O166" s="38" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="P166" s="38" t="s">
         <v>64</v>
@@ -11704,7 +11704,7 @@
       <c r="Q166" s="38"/>
       <c r="R166" s="38"/>
       <c r="S166" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T166" s="38" t="s">
         <v>226</v>
@@ -11735,13 +11735,13 @@
         <v>45960</v>
       </c>
       <c r="G167" s="37" t="s">
-        <v>599</v>
+        <v>587</v>
       </c>
       <c r="H167" s="37" t="s">
-        <v>600</v>
+        <v>588</v>
       </c>
       <c r="I167" s="42" t="s">
-        <v>601</v>
+        <v>589</v>
       </c>
       <c r="J167" s="38" t="s">
         <v>64</v>
@@ -11755,7 +11755,7 @@
         <v>64</v>
       </c>
       <c r="O167" s="38" t="s">
-        <v>602</v>
+        <v>590</v>
       </c>
       <c r="P167" s="38" t="s">
         <v>64</v>
@@ -11763,7 +11763,7 @@
       <c r="Q167" s="38"/>
       <c r="R167" s="38"/>
       <c r="S167" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T167" s="38" t="s">
         <v>226</v>
@@ -11794,13 +11794,13 @@
         <v>45960</v>
       </c>
       <c r="G168" s="37" t="s">
-        <v>603</v>
+        <v>591</v>
       </c>
       <c r="H168" s="37" t="s">
-        <v>604</v>
+        <v>592</v>
       </c>
       <c r="I168" s="42" t="s">
-        <v>605</v>
+        <v>593</v>
       </c>
       <c r="J168" s="38" t="s">
         <v>64</v>
@@ -11814,7 +11814,7 @@
         <v>64</v>
       </c>
       <c r="O168" s="38" t="s">
-        <v>606</v>
+        <v>594</v>
       </c>
       <c r="P168" s="38" t="s">
         <v>64</v>
@@ -11822,7 +11822,7 @@
       <c r="Q168" s="38"/>
       <c r="R168" s="38"/>
       <c r="S168" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T168" s="38" t="s">
         <v>226</v>
@@ -11853,13 +11853,13 @@
         <v>45960</v>
       </c>
       <c r="G169" s="37" t="s">
-        <v>607</v>
+        <v>595</v>
       </c>
       <c r="H169" s="37" t="s">
-        <v>608</v>
+        <v>596</v>
       </c>
       <c r="I169" s="42" t="s">
-        <v>609</v>
+        <v>597</v>
       </c>
       <c r="J169" s="38" t="s">
         <v>64</v>
@@ -11873,7 +11873,7 @@
         <v>64</v>
       </c>
       <c r="O169" s="38" t="s">
-        <v>610</v>
+        <v>598</v>
       </c>
       <c r="P169" s="38" t="s">
         <v>64</v>
@@ -11881,7 +11881,7 @@
       <c r="Q169" s="38"/>
       <c r="R169" s="38"/>
       <c r="S169" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T169" s="38" t="s">
         <v>226</v>
@@ -11912,13 +11912,13 @@
         <v>45960</v>
       </c>
       <c r="G170" s="37" t="s">
-        <v>611</v>
+        <v>599</v>
       </c>
       <c r="H170" s="37" t="s">
-        <v>612</v>
+        <v>600</v>
       </c>
       <c r="I170" s="42" t="s">
-        <v>613</v>
+        <v>601</v>
       </c>
       <c r="J170" s="38" t="s">
         <v>64</v>
@@ -11932,7 +11932,7 @@
         <v>64</v>
       </c>
       <c r="O170" s="38" t="s">
-        <v>614</v>
+        <v>602</v>
       </c>
       <c r="P170" s="38" t="s">
         <v>64</v>
@@ -11940,7 +11940,7 @@
       <c r="Q170" s="38"/>
       <c r="R170" s="38"/>
       <c r="S170" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T170" s="38" t="s">
         <v>226</v>
@@ -12230,13 +12230,13 @@
         <v>45960</v>
       </c>
       <c r="G178" s="37" t="s">
-        <v>615</v>
+        <v>603</v>
       </c>
       <c r="H178" s="37" t="s">
-        <v>616</v>
+        <v>604</v>
       </c>
       <c r="I178" s="37" t="s">
-        <v>617</v>
+        <v>605</v>
       </c>
       <c r="J178" s="38" t="s">
         <v>64</v>
@@ -12250,7 +12250,7 @@
         <v>64</v>
       </c>
       <c r="O178" s="38" t="s">
-        <v>618</v>
+        <v>606</v>
       </c>
       <c r="P178" s="38" t="s">
         <v>64</v>
@@ -12258,7 +12258,7 @@
       <c r="Q178" s="38"/>
       <c r="R178" s="38"/>
       <c r="S178" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T178" s="38" t="s">
         <v>226</v>
@@ -12289,13 +12289,13 @@
         <v>45960</v>
       </c>
       <c r="G179" s="37" t="s">
-        <v>619</v>
+        <v>607</v>
       </c>
       <c r="H179" s="37" t="s">
-        <v>620</v>
+        <v>608</v>
       </c>
       <c r="I179" s="37" t="s">
-        <v>621</v>
+        <v>609</v>
       </c>
       <c r="J179" s="38" t="s">
         <v>64</v>
@@ -12309,7 +12309,7 @@
         <v>64</v>
       </c>
       <c r="O179" s="38" t="s">
-        <v>622</v>
+        <v>610</v>
       </c>
       <c r="P179" s="38" t="s">
         <v>64</v>
@@ -12317,7 +12317,7 @@
       <c r="Q179" s="38"/>
       <c r="R179" s="38"/>
       <c r="S179" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T179" s="38" t="s">
         <v>226</v>
@@ -12459,13 +12459,13 @@
         <v>45960</v>
       </c>
       <c r="G183" s="37" t="s">
-        <v>623</v>
+        <v>611</v>
       </c>
       <c r="H183" s="37" t="s">
-        <v>624</v>
+        <v>612</v>
       </c>
       <c r="I183" s="37" t="s">
-        <v>625</v>
+        <v>613</v>
       </c>
       <c r="J183" s="38" t="s">
         <v>64</v>
@@ -12479,7 +12479,7 @@
         <v>64</v>
       </c>
       <c r="O183" s="38" t="s">
-        <v>626</v>
+        <v>614</v>
       </c>
       <c r="P183" s="38" t="s">
         <v>64</v>
@@ -12487,7 +12487,7 @@
       <c r="Q183" s="38"/>
       <c r="R183" s="38"/>
       <c r="S183" s="65" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T183" s="38" t="s">
         <v>226</v>
@@ -12518,13 +12518,13 @@
         <v>45960</v>
       </c>
       <c r="G184" s="37" t="s">
-        <v>630</v>
+        <v>618</v>
       </c>
       <c r="H184" s="37" t="s">
-        <v>631</v>
+        <v>619</v>
       </c>
       <c r="I184" s="37" t="s">
-        <v>632</v>
+        <v>620</v>
       </c>
       <c r="J184" s="38" t="s">
         <v>64</v>
@@ -12538,7 +12538,7 @@
         <v>64</v>
       </c>
       <c r="O184" s="38" t="s">
-        <v>633</v>
+        <v>621</v>
       </c>
       <c r="P184" s="38" t="s">
         <v>64</v>
@@ -12546,7 +12546,7 @@
       <c r="Q184" s="38"/>
       <c r="R184" s="38"/>
       <c r="S184" s="66" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T184" s="38" t="s">
         <v>226</v>
@@ -12577,13 +12577,13 @@
         <v>45960</v>
       </c>
       <c r="G185" s="37" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
       <c r="H185" s="37" t="s">
-        <v>635</v>
+        <v>623</v>
       </c>
       <c r="I185" s="37" t="s">
-        <v>636</v>
+        <v>624</v>
       </c>
       <c r="J185" s="38" t="s">
         <v>64</v>
@@ -12597,7 +12597,7 @@
         <v>64</v>
       </c>
       <c r="O185" s="38" t="s">
-        <v>637</v>
+        <v>625</v>
       </c>
       <c r="P185" s="38" t="s">
         <v>64</v>
@@ -12605,7 +12605,7 @@
       <c r="Q185" s="38"/>
       <c r="R185" s="38"/>
       <c r="S185" s="66" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T185" s="38" t="s">
         <v>226</v>
@@ -12710,13 +12710,13 @@
         <v>45807</v>
       </c>
       <c r="G188" s="37" t="s">
-        <v>647</v>
+        <v>635</v>
       </c>
       <c r="H188" s="37" t="s">
-        <v>648</v>
+        <v>636</v>
       </c>
       <c r="I188" s="42" t="s">
-        <v>649</v>
+        <v>637</v>
       </c>
       <c r="J188" s="38" t="s">
         <v>64</v>
@@ -12763,13 +12763,13 @@
         <v>45807</v>
       </c>
       <c r="G189" s="37" t="s">
-        <v>650</v>
+        <v>638</v>
       </c>
       <c r="H189" s="37" t="s">
-        <v>651</v>
+        <v>639</v>
       </c>
       <c r="I189" s="42" t="s">
-        <v>652</v>
+        <v>640</v>
       </c>
       <c r="J189" s="38" t="s">
         <v>64</v>
@@ -12816,13 +12816,13 @@
         <v>45807</v>
       </c>
       <c r="G190" s="35" t="s">
-        <v>638</v>
+        <v>626</v>
       </c>
       <c r="H190" s="38" t="s">
-        <v>639</v>
+        <v>627</v>
       </c>
       <c r="I190" s="45" t="s">
-        <v>640</v>
+        <v>628</v>
       </c>
       <c r="J190" s="38" t="s">
         <v>64</v>
@@ -12836,7 +12836,7 @@
         <v>64</v>
       </c>
       <c r="O190" s="38" t="s">
-        <v>641</v>
+        <v>629</v>
       </c>
       <c r="P190" s="38" t="s">
         <v>64</v>
@@ -12848,7 +12848,7 @@
         <v>64</v>
       </c>
       <c r="S190" s="66" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T190" s="38" t="s">
         <v>226</v>
@@ -12879,13 +12879,13 @@
         <v>45807</v>
       </c>
       <c r="G191" s="35" t="s">
-        <v>653</v>
+        <v>641</v>
       </c>
       <c r="H191" s="35" t="s">
-        <v>654</v>
+        <v>642</v>
       </c>
       <c r="I191" s="45" t="s">
-        <v>655</v>
+        <v>643</v>
       </c>
       <c r="J191" s="38" t="s">
         <v>64</v>
@@ -12899,7 +12899,7 @@
         <v>64</v>
       </c>
       <c r="O191" s="38" t="s">
-        <v>642</v>
+        <v>630</v>
       </c>
       <c r="P191" s="38" t="s">
         <v>64</v>
@@ -12907,7 +12907,7 @@
       <c r="Q191" s="38"/>
       <c r="R191" s="38"/>
       <c r="S191" s="66" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T191" s="38" t="s">
         <v>226</v>
@@ -12938,13 +12938,13 @@
         <v>45807</v>
       </c>
       <c r="G192" s="37" t="s">
-        <v>643</v>
+        <v>631</v>
       </c>
       <c r="H192" s="37" t="s">
-        <v>644</v>
+        <v>632</v>
       </c>
       <c r="I192" s="42" t="s">
-        <v>645</v>
+        <v>633</v>
       </c>
       <c r="J192" s="38" t="s">
         <v>64</v>
@@ -12958,7 +12958,7 @@
         <v>64</v>
       </c>
       <c r="O192" s="38" t="s">
-        <v>646</v>
+        <v>634</v>
       </c>
       <c r="P192" s="38" t="s">
         <v>64</v>
@@ -12966,7 +12966,7 @@
       <c r="Q192" s="38"/>
       <c r="R192" s="38"/>
       <c r="S192" s="66" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="T192" s="38" t="s">
         <v>226</v>
@@ -19289,27 +19289,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -19567,32 +19546,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACB08642-5694-4F88-BF6F-98521E3A5E0B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -19611,6 +19586,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{e0793d39-0939-496d-b129-198edd916feb}" enabled="0" method="" siteId="{e0793d39-0939-496d-b129-198edd916feb}" removed="1"/>

</xml_diff>